<commit_message>
AutoLoan AppData Entry Application Details Feature Commit
</commit_message>
<xml_diff>
--- a/Gowtham_ULS_New/TestData/ijaraTestData.xlsx
+++ b/Gowtham_ULS_New/TestData/ijaraTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="17" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ijara_LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -29,13 +29,14 @@
     <sheet name="ALAppdataEntryIncomedetails" sheetId="25" r:id="rId20"/>
     <sheet name="ALAppdataEntryDocumentsDetails" sheetId="26" r:id="rId21"/>
     <sheet name="AutoLoanExecution" sheetId="22" r:id="rId22"/>
+    <sheet name="RtALAppDataEntryApplicationDeta" sheetId="27" r:id="rId23"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="473">
   <si>
     <t>UserName</t>
   </si>
@@ -1426,18 +1427,6 @@
     <t>AT_AL_CUS_01_D1</t>
   </si>
   <si>
-    <t>AT_IJCS_01_D1</t>
-  </si>
-  <si>
-    <t>AT_IJCS_02_D1</t>
-  </si>
-  <si>
-    <t>AT_IJCS_03_D1</t>
-  </si>
-  <si>
-    <t>AT_IJCS_04_D1</t>
-  </si>
-  <si>
     <t>3050</t>
   </si>
   <si>
@@ -1445,6 +1434,27 @@
   </si>
   <si>
     <t>AT_Al_DOC_09_D1</t>
+  </si>
+  <si>
+    <t>DS_AT_IJCS_01</t>
+  </si>
+  <si>
+    <t>DS_AT_IJCS_02</t>
+  </si>
+  <si>
+    <t>DS_AT_IJCS_03</t>
+  </si>
+  <si>
+    <t>DS_AT_IJCS_04</t>
+  </si>
+  <si>
+    <t>AT_RD_ADE_AD_01</t>
+  </si>
+  <si>
+    <t>AT_RD_ADE_AD_01_D1</t>
+  </si>
+  <si>
+    <t>10:05</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1656,252 +1666,13 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2543,7 +2314,7 @@
         <v>250</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>63</v>
@@ -3173,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3261,8 +3032,8 @@
       <c r="G2" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="H2" s="17">
-        <v>0.4236111111111111</v>
+      <c r="H2" s="18" t="s">
+        <v>472</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>244</v>
@@ -3462,7 +3233,7 @@
         <v>445</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>278</v>
@@ -4378,8 +4149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4667,7 +4438,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4826,7 +4597,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4852,7 +4623,7 @@
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C2" s="17">
         <v>5301</v>
@@ -4867,8 +4638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4931,7 +4702,7 @@
         <v>438</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4942,7 +4713,7 @@
         <v>439</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4972,7 +4743,7 @@
         <v>442</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>426</v>
@@ -4983,7 +4754,7 @@
         <v>443</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>426</v>
@@ -5280,91 +5051,339 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C17">
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C17">
-    <cfRule type="cellIs" dxfId="35" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C14">
-    <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C25">
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C36">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C30">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C21">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C21">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C14">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C36">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="60" customHeight="1">
+      <c r="A1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="25">
+        <v>5301</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="17">
+        <v>9574315615</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="17">
+        <v>1234</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="T2" s="17">
+        <v>10000</v>
+      </c>
+      <c r="U2" s="17">
+        <v>10000</v>
+      </c>
+      <c r="V2" s="17">
+        <v>10000</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD2" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF2" s="17">
+        <v>10000</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5550,8 +5569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5626,7 +5645,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
@@ -5649,7 +5668,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -5681,7 +5700,7 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
@@ -5707,7 +5726,7 @@
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>

</xml_diff>